<commit_message>
Add similarity calculation module
- Implement similarity calculation module (similarity.py) with cosine similarity function
- Add support for finding top N most similar items based on vector representations
- Update README.md with Phase 2 changes, including new module documentation and usage examples
- Add text2vec to required dependencies in installation instructions

This commit enhances the product recommendation system by implementing a core similarity calculation functionality that will be used in the collaborative filtering module to find similar products based on their vector representations.
</commit_message>
<xml_diff>
--- a/sales.xlsx
+++ b/sales.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\course\2cLesson\SiyuanWang\ProductRecommendation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\course\2cLesson\SiyuanWang\ProductRecommendation\github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF0C12-D618-4453-938D-C88F79793D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF68809-234B-4102-90CA-6586C2599455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="224">
   <si>
     <t>customer_id</t>
   </si>
@@ -58,432 +58,243 @@
     <t>C1001</t>
   </si>
   <si>
-    <t>张伟</t>
-  </si>
-  <si>
     <t>O202507151</t>
   </si>
   <si>
     <t>P2001</t>
   </si>
   <si>
-    <t>男士T恤</t>
-  </si>
-  <si>
-    <t>男装</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>P3105</t>
   </si>
   <si>
-    <t>休闲短裤</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>O202508012</t>
   </si>
   <si>
     <t>P4502</t>
   </si>
   <si>
-    <t>运动鞋</t>
-  </si>
-  <si>
-    <t>鞋类</t>
-  </si>
-  <si>
     <t>C1002</t>
   </si>
   <si>
-    <t>李娜</t>
-  </si>
-  <si>
     <t>O202507221</t>
   </si>
   <si>
     <t>P1180</t>
   </si>
   <si>
-    <t>碎花连衣裙</t>
-  </si>
-  <si>
-    <t>女装</t>
-  </si>
-  <si>
     <t>P7601</t>
   </si>
   <si>
-    <t>时尚太阳镜</t>
-  </si>
-  <si>
-    <t>配饰</t>
-  </si>
-  <si>
-    <t>均码</t>
-  </si>
-  <si>
     <t>C1003</t>
   </si>
   <si>
-    <t>王雷</t>
-  </si>
-  <si>
     <t>O202508103</t>
   </si>
   <si>
-    <t>XL</t>
-  </si>
-  <si>
     <t>O202507284</t>
   </si>
   <si>
     <t>P3210</t>
   </si>
   <si>
-    <t>工装裤</t>
-  </si>
-  <si>
     <t>C1004</t>
   </si>
   <si>
-    <t>刘芳</t>
-  </si>
-  <si>
     <t>O202506155</t>
   </si>
   <si>
     <t>P1305</t>
   </si>
   <si>
-    <t>V领针织衫</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>O202507186</t>
   </si>
   <si>
     <t>P6507</t>
   </si>
   <si>
-    <t>尖头高跟鞋</t>
-  </si>
-  <si>
     <t>C1005</t>
   </si>
   <si>
-    <t>陈明</t>
-  </si>
-  <si>
     <t>O202508067</t>
   </si>
   <si>
     <t>P5203</t>
   </si>
   <si>
-    <t>牛仔外套</t>
-  </si>
-  <si>
     <t>O202507219</t>
   </si>
   <si>
     <t>P7703</t>
   </si>
   <si>
-    <t>皮质腰带</t>
-  </si>
-  <si>
     <t>C1006</t>
   </si>
   <si>
-    <t>赵静</t>
-  </si>
-  <si>
     <t>O202506305</t>
   </si>
   <si>
     <t>P1508</t>
   </si>
   <si>
-    <t>雪纺连衣裙</t>
-  </si>
-  <si>
     <t>O202507248</t>
   </si>
   <si>
     <t>P8809</t>
   </si>
   <si>
-    <t>真丝衬衫</t>
-  </si>
-  <si>
     <t>P9204</t>
   </si>
   <si>
-    <t>水晶耳环</t>
-  </si>
-  <si>
     <t>C1007</t>
   </si>
   <si>
-    <t>杨洋</t>
-  </si>
-  <si>
     <t>O202506217</t>
   </si>
   <si>
     <t>P2407</t>
   </si>
   <si>
-    <t>连帽卫衣</t>
-  </si>
-  <si>
     <t>O202507289</t>
   </si>
   <si>
     <t>P6703</t>
   </si>
   <si>
-    <t>系带乐福鞋</t>
-  </si>
-  <si>
     <t>C1008</t>
   </si>
   <si>
-    <t>孙梅</t>
-  </si>
-  <si>
     <t>O202506184</t>
   </si>
   <si>
     <t>P1120</t>
   </si>
   <si>
-    <t>蕾丝上衣</t>
-  </si>
-  <si>
     <t>O202507231</t>
   </si>
   <si>
     <t>P6305</t>
   </si>
   <si>
-    <t>帆布鞋</t>
-  </si>
-  <si>
     <t>C1009</t>
   </si>
   <si>
-    <t>周强</t>
-  </si>
-  <si>
     <t>O202507191</t>
   </si>
   <si>
     <t>P2908</t>
   </si>
   <si>
-    <t>西服套装</t>
-  </si>
-  <si>
     <t>C1010</t>
   </si>
   <si>
-    <t>吴霞</t>
-  </si>
-  <si>
     <t>O202508109</t>
   </si>
   <si>
     <t>P1703</t>
   </si>
   <si>
-    <t>阔腿裤</t>
-  </si>
-  <si>
     <t>C1011</t>
   </si>
   <si>
-    <t>郑凯</t>
-  </si>
-  <si>
     <t>O202507264</t>
   </si>
   <si>
     <t>P3802</t>
   </si>
   <si>
-    <t>速干运动裤</t>
-  </si>
-  <si>
     <t>P5601</t>
   </si>
   <si>
-    <t>羊毛大衣</t>
-  </si>
-  <si>
     <t>C1012</t>
   </si>
   <si>
-    <t>林婷</t>
-  </si>
-  <si>
     <t>O202506257</t>
   </si>
   <si>
     <t>P1406</t>
   </si>
   <si>
-    <t>旗袍</t>
-  </si>
-  <si>
     <t>P9108</t>
   </si>
   <si>
-    <t>珍珠项链</t>
-  </si>
-  <si>
     <t>C1013</t>
   </si>
   <si>
-    <t>黄超</t>
-  </si>
-  <si>
     <t>O202507301</t>
   </si>
   <si>
     <t>P2505</t>
   </si>
   <si>
-    <t>POLO衫</t>
-  </si>
-  <si>
     <t>P3301</t>
   </si>
   <si>
-    <t>休闲皮鞋</t>
-  </si>
-  <si>
     <t>C1014</t>
   </si>
   <si>
-    <t>徐薇</t>
-  </si>
-  <si>
     <t>O202507208</t>
   </si>
   <si>
     <t>P1602</t>
   </si>
   <si>
-    <t>针织开衫</t>
-  </si>
-  <si>
     <t>C1015</t>
   </si>
   <si>
-    <t>陈思思</t>
-  </si>
-  <si>
     <t>O202507311</t>
   </si>
   <si>
     <t>O202508119</t>
   </si>
   <si>
-    <t>高跟鞋</t>
-  </si>
-  <si>
     <t>C1016</t>
   </si>
   <si>
-    <t>高翔</t>
-  </si>
-  <si>
     <t>O202507225</t>
   </si>
   <si>
     <t>P2609</t>
   </si>
   <si>
-    <t>风衣外套</t>
-  </si>
-  <si>
     <t>P4103</t>
   </si>
   <si>
-    <t>运动裤</t>
-  </si>
-  <si>
     <t>C1017</t>
   </si>
   <si>
-    <t>谢芳</t>
-  </si>
-  <si>
     <t>O202506209</t>
   </si>
   <si>
     <t>P1208</t>
   </si>
   <si>
-    <t>雪纺衬衫</t>
-  </si>
-  <si>
     <t>O202507267</t>
   </si>
   <si>
     <t>P9402</t>
   </si>
   <si>
-    <t>丝巾</t>
-  </si>
-  <si>
     <t>C1018</t>
   </si>
   <si>
-    <t>邓伟</t>
-  </si>
-  <si>
     <t>O202506245</t>
   </si>
   <si>
     <t>P2703</t>
   </si>
   <si>
-    <t>羽绒服</t>
-  </si>
-  <si>
-    <t>XXL</t>
-  </si>
-  <si>
     <t>C1019</t>
   </si>
   <si>
-    <t>汪敏</t>
-  </si>
-  <si>
     <t>O202507274</t>
   </si>
   <si>
     <t>P1805</t>
   </si>
   <si>
-    <t>半身裙</t>
-  </si>
-  <si>
     <t>C1020</t>
   </si>
   <si>
-    <t>叶鹏</t>
-  </si>
-  <si>
     <t>O202508014</t>
   </si>
   <si>
@@ -493,184 +304,394 @@
     <t>P3404</t>
   </si>
   <si>
-    <t>马丁靴</t>
-  </si>
-  <si>
     <t>C1021</t>
   </si>
   <si>
-    <t>魏琳</t>
-  </si>
-  <si>
     <t>O202507212</t>
   </si>
   <si>
     <t>P1903</t>
   </si>
   <si>
-    <t>牛仔短裤</t>
-  </si>
-  <si>
     <t>P7502</t>
   </si>
   <si>
-    <t>时尚手表</t>
-  </si>
-  <si>
     <t>C1022</t>
   </si>
   <si>
-    <t>潘阳</t>
-  </si>
-  <si>
     <t>O202508116</t>
   </si>
   <si>
     <t>P4301</t>
   </si>
   <si>
-    <t>休闲板鞋</t>
-  </si>
-  <si>
     <t>C1023</t>
   </si>
   <si>
-    <t>夏雪</t>
-  </si>
-  <si>
     <t>O202506235</t>
   </si>
   <si>
     <t>C1024</t>
   </si>
   <si>
-    <t>崔亮</t>
-  </si>
-  <si>
     <t>O202507251</t>
   </si>
   <si>
     <t>P3007</t>
   </si>
   <si>
-    <t>哈伦裤</t>
-  </si>
-  <si>
     <t>P7205</t>
   </si>
   <si>
-    <t>皮质钱包</t>
-  </si>
-  <si>
     <t>C1025</t>
   </si>
   <si>
-    <t>薛婷</t>
-  </si>
-  <si>
     <t>O202508122</t>
   </si>
   <si>
     <t>P9603</t>
   </si>
   <si>
-    <t>贝雷帽</t>
-  </si>
-  <si>
     <t>C1026</t>
   </si>
   <si>
-    <t>毛伟</t>
-  </si>
-  <si>
     <t>O202507297</t>
   </si>
   <si>
     <t>P2209</t>
   </si>
   <si>
-    <t>条纹衬衫</t>
-  </si>
-  <si>
     <t>C1027</t>
   </si>
   <si>
-    <t>韩雪</t>
-  </si>
-  <si>
     <t>O202507255</t>
   </si>
   <si>
     <t>P8501</t>
   </si>
   <si>
-    <t>蕾丝连衣裙</t>
-  </si>
-  <si>
     <t>C1028</t>
   </si>
   <si>
-    <t>赵志强</t>
-  </si>
-  <si>
     <t>O202506205</t>
   </si>
   <si>
     <t>P5305</t>
   </si>
   <si>
-    <t>夹克外套</t>
-  </si>
-  <si>
     <t>O202507226</t>
   </si>
   <si>
     <t>P8007</t>
   </si>
   <si>
-    <t>职业套装</t>
-  </si>
-  <si>
     <t>C1029</t>
   </si>
   <si>
-    <t>郭琳</t>
-  </si>
-  <si>
     <t>O202506272</t>
   </si>
   <si>
     <t>P7304</t>
   </si>
   <si>
-    <t>太阳帽</t>
-  </si>
-  <si>
     <t>C1030</t>
   </si>
   <si>
-    <t>林浩</t>
-  </si>
-  <si>
     <t>O202507242</t>
   </si>
   <si>
     <t>P3603</t>
   </si>
   <si>
-    <t>休闲凉鞋</t>
-  </si>
-  <si>
     <t>O202508131</t>
   </si>
   <si>
     <t>P5102</t>
   </si>
   <si>
-    <t>牛仔裤</t>
-  </si>
-  <si>
     <t>product_category</t>
+  </si>
+  <si>
+    <t>张伟 (Zhang Wei)</t>
+  </si>
+  <si>
+    <t>李娜 (Li Na)</t>
+  </si>
+  <si>
+    <t>王雷 (Wang Lei)</t>
+  </si>
+  <si>
+    <t>刘芳 (Liu Fang)</t>
+  </si>
+  <si>
+    <t>陈明 (Chen Ming)</t>
+  </si>
+  <si>
+    <t>赵静 (Zhao Jing)</t>
+  </si>
+  <si>
+    <t>杨洋 (Yang Yang)</t>
+  </si>
+  <si>
+    <t>孙梅 (Sun Mei)</t>
+  </si>
+  <si>
+    <t>周强 (Zhou Qiang)</t>
+  </si>
+  <si>
+    <t>吴霞 (Wu Xia)</t>
+  </si>
+  <si>
+    <t>郑凯 (Zheng Kai)</t>
+  </si>
+  <si>
+    <t>林婷 (Lin Ting)</t>
+  </si>
+  <si>
+    <t>黄超 (Huang Chao)</t>
+  </si>
+  <si>
+    <t>徐薇 (Xu Wei)</t>
+  </si>
+  <si>
+    <t>陈思思 (Chen Sisi)</t>
+  </si>
+  <si>
+    <t>高翔 (Gao Xiang)</t>
+  </si>
+  <si>
+    <t>谢芳 (Xie Fang)</t>
+  </si>
+  <si>
+    <t>邓伟 (Deng Wei)</t>
+  </si>
+  <si>
+    <t>汪敏 (Wang Min)</t>
+  </si>
+  <si>
+    <t>叶鹏 (Ye Peng)</t>
+  </si>
+  <si>
+    <t>魏琳 (Wei Lin)</t>
+  </si>
+  <si>
+    <t>潘阳 (Pan Yang)</t>
+  </si>
+  <si>
+    <t>夏雪 (Xia Xue)</t>
+  </si>
+  <si>
+    <t>崔亮 (Cui Liang)</t>
+  </si>
+  <si>
+    <t>薛婷 (Xue Ting)</t>
+  </si>
+  <si>
+    <t>毛伟 (Mao Wei)</t>
+  </si>
+  <si>
+    <t>韩雪 (Han Xue)</t>
+  </si>
+  <si>
+    <t>赵志强 (Zhao Zhiqiang)</t>
+  </si>
+  <si>
+    <t>郭琳 (Guo Lin)</t>
+  </si>
+  <si>
+    <t>林浩 (Lin Hao)</t>
+  </si>
+  <si>
+    <t>男士T恤 (Men’s T-shirt)</t>
+  </si>
+  <si>
+    <t>休闲短裤 (Casual Shorts)</t>
+  </si>
+  <si>
+    <t>运动鞋 (Sneakers)</t>
+  </si>
+  <si>
+    <t>碎花连衣裙 (Floral Dress)</t>
+  </si>
+  <si>
+    <t>时尚太阳镜 (Fashion Sunglasses)</t>
+  </si>
+  <si>
+    <t>工装裤 (Cargo Pants)</t>
+  </si>
+  <si>
+    <t>V领针织衫 (V-neck Sweater)</t>
+  </si>
+  <si>
+    <t>尖头高跟鞋 (Stilettos)</t>
+  </si>
+  <si>
+    <t>牛仔外套 (Denim Jacket)</t>
+  </si>
+  <si>
+    <t>皮质腰带 (Leather Belt)</t>
+  </si>
+  <si>
+    <t>雪纺连衣裙 (Chiffon Dress)</t>
+  </si>
+  <si>
+    <t>真丝衬衫 (Silk Blouse)</t>
+  </si>
+  <si>
+    <t>水晶耳环 (Crystal Earrings)</t>
+  </si>
+  <si>
+    <t>连帽卫衣 (Hoodie)</t>
+  </si>
+  <si>
+    <t>系带乐福鞋 (Loafers)</t>
+  </si>
+  <si>
+    <t>蕾丝上衣 (Lace Top)</t>
+  </si>
+  <si>
+    <t>帆布鞋 (Canvas Shoes)</t>
+  </si>
+  <si>
+    <t>西服套装 (Suit Set)</t>
+  </si>
+  <si>
+    <t>阔腿裤 (Wide-leg Pants)</t>
+  </si>
+  <si>
+    <t>速干运动裤 (Quick-dry Sports Pants)</t>
+  </si>
+  <si>
+    <t>羊毛大衣 (Wool Coat)</t>
+  </si>
+  <si>
+    <t>旗袍 (Qipao / Cheongsam)</t>
+  </si>
+  <si>
+    <t>珍珠项链 (Pearl Necklace)</t>
+  </si>
+  <si>
+    <t>POLO衫 (Polo Shirt)</t>
+  </si>
+  <si>
+    <t>休闲皮鞋 (Casual Leather Shoes)</t>
+  </si>
+  <si>
+    <t>针织开衫 (Cardigan)</t>
+  </si>
+  <si>
+    <t>高跟鞋 (High Heels)</t>
+  </si>
+  <si>
+    <t>风衣外套 (Trench Coat)</t>
+  </si>
+  <si>
+    <t>运动裤 (Sports Pants)</t>
+  </si>
+  <si>
+    <t>雪纺衬衫 (Chiffon Blouse)</t>
+  </si>
+  <si>
+    <t>丝巾 (Silk Scarf)</t>
+  </si>
+  <si>
+    <t>羽绒服 (Down Jacket)</t>
+  </si>
+  <si>
+    <t>半身裙 (Skirt)</t>
+  </si>
+  <si>
+    <t>马丁靴 (Martin Boots)</t>
+  </si>
+  <si>
+    <t>牛仔短裤 (Denim Shorts)</t>
+  </si>
+  <si>
+    <t>时尚手表 (Fashion Watch)</t>
+  </si>
+  <si>
+    <t>休闲板鞋 (Casual Skate Shoes)</t>
+  </si>
+  <si>
+    <t>哈伦裤 (Harem Pants)</t>
+  </si>
+  <si>
+    <t>皮质钱包 (Leather Wallet)</t>
+  </si>
+  <si>
+    <t>贝雷帽 (Beret)</t>
+  </si>
+  <si>
+    <t>条纹衬衫 (Striped Shirt)</t>
+  </si>
+  <si>
+    <t>蕾丝连衣裙 (Lace Dress)</t>
+  </si>
+  <si>
+    <t>夹克外套 (Jacket)</t>
+  </si>
+  <si>
+    <t>职业套装 (Business Suit)</t>
+  </si>
+  <si>
+    <t>太阳帽 (Sun Hat)</t>
+  </si>
+  <si>
+    <t>休闲凉鞋 (Casual Sandals)</t>
+  </si>
+  <si>
+    <t>牛仔裤 (Jeans)</t>
+  </si>
+  <si>
+    <t>男装 (Men’s Clothing)</t>
+  </si>
+  <si>
+    <t>鞋类 (Footwear)</t>
+  </si>
+  <si>
+    <t>女装 (Women’s Clothing)</t>
+  </si>
+  <si>
+    <t>配饰 (Accessories)</t>
+  </si>
+  <si>
+    <t>M (Medium)</t>
+  </si>
+  <si>
+    <t>L (Large)</t>
+  </si>
+  <si>
+    <t>42 (Size 42)</t>
+  </si>
+  <si>
+    <t>均码 (Free Size)</t>
+  </si>
+  <si>
+    <t>XL (Extra Large)</t>
+  </si>
+  <si>
+    <t>S (Small)</t>
+  </si>
+  <si>
+    <t>37 (Size 37)</t>
+  </si>
+  <si>
+    <t>43 (Size 43)</t>
+  </si>
+  <si>
+    <t>38 (Size 38)</t>
+  </si>
+  <si>
+    <t>44 (Size 44)</t>
+  </si>
+  <si>
+    <t>XXL (Extra Extra Large)</t>
+  </si>
+  <si>
+    <t>41 (Size 41)</t>
+  </si>
+  <si>
+    <t>32 (Size 32)</t>
   </si>
 </sst>
 </file>
@@ -680,7 +701,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +721,12 @@
       <color rgb="FFA31515"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1A2029"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -724,7 +751,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -732,6 +759,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1076,7 +1106,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H2" sqref="H2:H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1134,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>216</v>
+        <v>129</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -1126,26 +1156,26 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
+      <c r="B2" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C2">
         <v>13800111234</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
+      <c r="F2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I2">
         <v>199</v>
@@ -1164,26 +1194,26 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
+      <c r="B3" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C3">
         <v>13800111234</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I3">
         <v>299</v>
@@ -1202,26 +1232,26 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="B4" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C4">
         <v>13800111234</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4">
-        <v>42</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="I4">
         <v>899</v>
@@ -1238,28 +1268,28 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C5">
         <v>15900225678</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I5">
         <v>599</v>
@@ -1276,28 +1306,28 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C6">
         <v>15900225678</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I6">
         <v>399</v>
@@ -1314,28 +1344,28 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C7">
         <v>18600339012</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="I7">
         <v>199</v>
@@ -1352,28 +1382,28 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C8">
         <v>18600339012</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I8">
         <v>459</v>
@@ -1390,28 +1420,28 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C9">
         <v>13500443344</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="I9">
         <v>389</v>
@@ -1428,28 +1458,28 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C10">
         <v>13500443344</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="I10">
         <v>1199</v>
@@ -1466,28 +1496,28 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C11">
         <v>18800557665</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I11">
         <v>659</v>
@@ -1504,28 +1534,28 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C12">
         <v>18800557665</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" t="s">
         <v>34</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I12">
         <v>289</v>
@@ -1542,28 +1572,28 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C13">
         <v>13700669876</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I13">
         <v>729</v>
@@ -1580,28 +1610,28 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C14">
         <v>13700669876</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
+        <v>39</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I14">
         <v>689</v>
@@ -1618,28 +1648,28 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" t="s">
-        <v>60</v>
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C15">
         <v>13700669876</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I15">
         <v>199</v>
@@ -1656,28 +1686,28 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
+        <v>41</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C16">
         <v>13900771188</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="I16">
         <v>359</v>
@@ -1694,28 +1724,28 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
+        <v>41</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C17">
         <v>13900771188</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="I17">
         <v>1299</v>
@@ -1732,28 +1762,28 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" t="s">
-        <v>78</v>
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C18">
         <v>15800882299</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="I18">
         <v>419</v>
@@ -1770,28 +1800,28 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>78</v>
+        <v>46</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C19">
         <v>15800882299</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="I19">
         <v>499</v>
@@ -1808,28 +1838,28 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" t="s">
-        <v>86</v>
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="C20">
         <v>18200993300</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" t="s">
-        <v>20</v>
+        <v>53</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I20">
         <v>1599</v>
@@ -1846,28 +1876,28 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" t="s">
-        <v>91</v>
+        <v>54</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="C21">
         <v>13601004411</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" t="s">
-        <v>17</v>
+        <v>56</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I21">
         <v>489</v>
@@ -1884,28 +1914,28 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" t="s">
-        <v>96</v>
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="C22">
         <v>18901115522</v>
       </c>
       <c r="D22" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" t="s">
-        <v>17</v>
+        <v>59</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I22">
         <v>329</v>
@@ -1922,28 +1952,28 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" t="s">
-        <v>96</v>
+        <v>57</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="C23">
         <v>18901115522</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" t="s">
-        <v>38</v>
+        <v>60</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="I23">
         <v>899</v>
@@ -1960,28 +1990,28 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="C24">
         <v>13101226633</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I24">
         <v>1399</v>
@@ -1998,28 +2028,28 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="C25">
         <v>13101226633</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
-      </c>
-      <c r="F25" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" t="s">
-        <v>34</v>
+        <v>64</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I25">
         <v>899</v>
@@ -2036,28 +2066,28 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
+        <v>65</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="C26">
         <v>18501337744</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" t="s">
-        <v>113</v>
-      </c>
-      <c r="G26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" t="s">
-        <v>20</v>
+        <v>67</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I26">
         <v>279</v>
@@ -2074,28 +2104,28 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" t="s">
-        <v>110</v>
+        <v>65</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="C27">
         <v>18501337744</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27">
-        <v>44</v>
+        <v>68</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="I27">
         <v>799</v>
@@ -2112,28 +2142,28 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" t="s">
-        <v>117</v>
+        <v>69</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="C28">
         <v>15001448855</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" t="s">
-        <v>120</v>
-      </c>
-      <c r="G28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" t="s">
-        <v>20</v>
+        <v>71</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I28">
         <v>559</v>
@@ -2150,28 +2180,28 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" t="s">
-        <v>122</v>
+        <v>72</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="C29">
         <v>13501553344</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" t="s">
-        <v>17</v>
+        <v>39</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I29">
         <v>689</v>
@@ -2188,28 +2218,28 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" t="s">
-        <v>122</v>
+        <v>72</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="C30">
         <v>13501553344</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" t="s">
-        <v>125</v>
-      </c>
-      <c r="G30" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="I30">
         <v>1299</v>
@@ -2226,28 +2256,28 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" t="s">
-        <v>127</v>
+        <v>75</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C31">
         <v>18601664477</v>
       </c>
       <c r="D31" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G31" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" t="s">
-        <v>38</v>
+        <v>77</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="I31">
         <v>799</v>
@@ -2264,28 +2294,28 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" t="s">
-        <v>127</v>
+        <v>75</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C32">
         <v>18601664477</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
-      </c>
-      <c r="F32" t="s">
-        <v>132</v>
-      </c>
-      <c r="G32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" t="s">
-        <v>20</v>
+        <v>78</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I32">
         <v>419</v>
@@ -2302,28 +2332,28 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>133</v>
-      </c>
-      <c r="B33" t="s">
-        <v>134</v>
+        <v>79</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="C33">
         <v>13301775588</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" t="s">
-        <v>137</v>
-      </c>
-      <c r="G33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" t="s">
-        <v>17</v>
+        <v>81</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I33">
         <v>359</v>
@@ -2340,28 +2370,28 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" t="s">
-        <v>134</v>
+        <v>79</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="C34">
         <v>13301775588</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="E34" t="s">
-        <v>139</v>
-      </c>
-      <c r="F34" t="s">
-        <v>140</v>
-      </c>
-      <c r="G34" t="s">
-        <v>33</v>
-      </c>
-      <c r="H34" t="s">
-        <v>34</v>
+        <v>83</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I34">
         <v>159</v>
@@ -2378,28 +2408,28 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>141</v>
-      </c>
-      <c r="B35" t="s">
-        <v>142</v>
+        <v>84</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="C35">
         <v>18001886699</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>144</v>
-      </c>
-      <c r="F35" t="s">
-        <v>145</v>
-      </c>
-      <c r="G35" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" t="s">
-        <v>146</v>
+        <v>86</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="I35">
         <v>1299</v>
@@ -2416,28 +2446,28 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C36">
         <v>15701997700</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
-      </c>
-      <c r="F36" t="s">
-        <v>151</v>
-      </c>
-      <c r="G36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" t="s">
-        <v>47</v>
+        <v>89</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="I36">
         <v>319</v>
@@ -2454,28 +2484,28 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>152</v>
-      </c>
-      <c r="B37" t="s">
-        <v>153</v>
+        <v>90</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C37">
         <v>18802008811</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="I37">
         <v>899</v>
@@ -2492,28 +2522,28 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>152</v>
-      </c>
-      <c r="B38" t="s">
-        <v>153</v>
+        <v>90</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C38">
         <v>18802008811</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>92</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
-      </c>
-      <c r="F38" t="s">
-        <v>157</v>
-      </c>
-      <c r="G38" t="s">
-        <v>24</v>
-      </c>
-      <c r="H38">
-        <v>43</v>
+        <v>93</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="I38">
         <v>999</v>
@@ -2530,28 +2560,28 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" t="s">
-        <v>159</v>
+        <v>94</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="C39">
         <v>13402119922</v>
       </c>
       <c r="D39" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>161</v>
-      </c>
-      <c r="F39" t="s">
-        <v>162</v>
-      </c>
-      <c r="G39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" t="s">
-        <v>17</v>
+        <v>96</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I39">
         <v>289</v>
@@ -2568,28 +2598,28 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>158</v>
-      </c>
-      <c r="B40" t="s">
-        <v>159</v>
+        <v>94</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="C40">
         <v>13402119922</v>
       </c>
       <c r="D40" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="E40" t="s">
-        <v>163</v>
-      </c>
-      <c r="F40" t="s">
-        <v>164</v>
-      </c>
-      <c r="G40" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" t="s">
-        <v>34</v>
+        <v>97</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I40">
         <v>699</v>
@@ -2606,28 +2636,28 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>165</v>
-      </c>
-      <c r="B41" t="s">
-        <v>166</v>
+        <v>98</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="C41">
         <v>18102221133</v>
       </c>
       <c r="D41" t="s">
-        <v>167</v>
+        <v>99</v>
       </c>
       <c r="E41" t="s">
-        <v>168</v>
-      </c>
-      <c r="F41" t="s">
-        <v>169</v>
-      </c>
-      <c r="G41" t="s">
-        <v>24</v>
-      </c>
-      <c r="H41">
-        <v>42</v>
+        <v>100</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="I41">
         <v>659</v>
@@ -2644,28 +2674,28 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>170</v>
-      </c>
-      <c r="B42" t="s">
-        <v>171</v>
+        <v>101</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C42">
         <v>15602332244</v>
       </c>
       <c r="D42" t="s">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I42">
         <v>389</v>
@@ -2682,28 +2712,28 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>173</v>
-      </c>
-      <c r="B43" t="s">
-        <v>174</v>
+        <v>103</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C43">
         <v>18202443355</v>
       </c>
       <c r="D43" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="E43" t="s">
-        <v>176</v>
-      </c>
-      <c r="F43" t="s">
-        <v>177</v>
-      </c>
-      <c r="G43" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" t="s">
-        <v>17</v>
+        <v>105</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I43">
         <v>389</v>
@@ -2720,28 +2750,28 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44" t="s">
-        <v>174</v>
+        <v>103</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C44">
         <v>18202443355</v>
       </c>
       <c r="D44" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="E44" t="s">
-        <v>178</v>
-      </c>
-      <c r="F44" t="s">
-        <v>179</v>
-      </c>
-      <c r="G44" t="s">
-        <v>33</v>
-      </c>
-      <c r="H44" t="s">
-        <v>34</v>
+        <v>106</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I44">
         <v>499</v>
@@ -2758,28 +2788,28 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>180</v>
-      </c>
-      <c r="B45" t="s">
-        <v>181</v>
+        <v>107</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C45">
         <v>13502554466</v>
       </c>
       <c r="D45" t="s">
-        <v>182</v>
+        <v>108</v>
       </c>
       <c r="E45" t="s">
-        <v>183</v>
-      </c>
-      <c r="F45" t="s">
-        <v>184</v>
-      </c>
-      <c r="G45" t="s">
-        <v>33</v>
-      </c>
-      <c r="H45" t="s">
-        <v>34</v>
+        <v>109</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I45">
         <v>229</v>
@@ -2796,28 +2826,28 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>185</v>
-      </c>
-      <c r="B46" t="s">
-        <v>186</v>
+        <v>110</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C46">
         <v>18702665577</v>
       </c>
       <c r="D46" t="s">
-        <v>187</v>
+        <v>111</v>
       </c>
       <c r="E46" t="s">
-        <v>188</v>
-      </c>
-      <c r="F46" t="s">
-        <v>189</v>
-      </c>
-      <c r="G46" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" t="s">
-        <v>20</v>
+        <v>112</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I46">
         <v>459</v>
@@ -2834,28 +2864,28 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>190</v>
-      </c>
-      <c r="B47" t="s">
-        <v>191</v>
+        <v>113</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="C47">
         <v>13002776688</v>
       </c>
       <c r="D47" t="s">
-        <v>192</v>
+        <v>114</v>
       </c>
       <c r="E47" t="s">
-        <v>105</v>
-      </c>
-      <c r="F47" t="s">
-        <v>106</v>
-      </c>
-      <c r="G47" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" t="s">
-        <v>47</v>
+        <v>63</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="I47">
         <v>1399</v>
@@ -2872,28 +2902,28 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>190</v>
-      </c>
-      <c r="B48" t="s">
-        <v>191</v>
+        <v>113</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="C48">
         <v>13002776688</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>114</v>
       </c>
       <c r="E48" t="s">
-        <v>193</v>
-      </c>
-      <c r="F48" t="s">
-        <v>194</v>
-      </c>
-      <c r="G48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H48" t="s">
-        <v>17</v>
+        <v>115</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I48">
         <v>789</v>
@@ -2910,28 +2940,28 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>195</v>
-      </c>
-      <c r="B49" t="s">
-        <v>196</v>
+        <v>116</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C49">
         <v>18802887766</v>
       </c>
       <c r="D49" t="s">
-        <v>197</v>
+        <v>117</v>
       </c>
       <c r="E49" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" t="s">
-        <v>146</v>
+        <v>13</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="I49">
         <v>199</v>
@@ -2948,28 +2978,28 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>195</v>
-      </c>
-      <c r="B50" t="s">
-        <v>196</v>
+        <v>116</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C50">
         <v>18802887766</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
-        <v>198</v>
-      </c>
-      <c r="F50" t="s">
-        <v>199</v>
-      </c>
-      <c r="G50" t="s">
-        <v>16</v>
-      </c>
-      <c r="H50" t="s">
-        <v>38</v>
+        <v>118</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="I50">
         <v>729</v>
@@ -2986,28 +3016,28 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" t="s">
-        <v>196</v>
+        <v>116</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C51">
         <v>18802887766</v>
       </c>
       <c r="D51" t="s">
-        <v>200</v>
+        <v>119</v>
       </c>
       <c r="E51" t="s">
-        <v>201</v>
-      </c>
-      <c r="F51" t="s">
-        <v>202</v>
-      </c>
-      <c r="G51" t="s">
-        <v>30</v>
-      </c>
-      <c r="H51" t="s">
-        <v>20</v>
+        <v>120</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="I51">
         <v>1199</v>
@@ -3024,28 +3054,28 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" t="s">
-        <v>204</v>
+        <v>121</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C52">
         <v>15902998899</v>
       </c>
       <c r="D52" t="s">
-        <v>205</v>
+        <v>122</v>
       </c>
       <c r="E52" t="s">
-        <v>93</v>
-      </c>
-      <c r="F52" t="s">
-        <v>94</v>
-      </c>
-      <c r="G52" t="s">
-        <v>30</v>
-      </c>
-      <c r="H52" t="s">
-        <v>17</v>
+        <v>56</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="I52">
         <v>489</v>
@@ -3062,28 +3092,28 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>203</v>
-      </c>
-      <c r="B53" t="s">
-        <v>204</v>
+        <v>121</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C53">
         <v>15902998899</v>
       </c>
       <c r="D53" t="s">
-        <v>205</v>
+        <v>122</v>
       </c>
       <c r="E53" t="s">
-        <v>206</v>
-      </c>
-      <c r="F53" t="s">
-        <v>207</v>
-      </c>
-      <c r="G53" t="s">
-        <v>33</v>
-      </c>
-      <c r="H53" t="s">
-        <v>34</v>
+        <v>123</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="I53">
         <v>189</v>
@@ -3100,28 +3130,28 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>208</v>
-      </c>
-      <c r="B54" t="s">
-        <v>209</v>
+        <v>124</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C54">
         <v>13703009900</v>
       </c>
       <c r="D54" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="E54" t="s">
-        <v>211</v>
-      </c>
-      <c r="F54" t="s">
-        <v>212</v>
-      </c>
-      <c r="G54" t="s">
-        <v>24</v>
-      </c>
-      <c r="H54">
-        <v>44</v>
+        <v>126</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="I54">
         <v>559</v>
@@ -3138,28 +3168,28 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>208</v>
-      </c>
-      <c r="B55" t="s">
-        <v>209</v>
+        <v>124</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C55">
         <v>13703009900</v>
       </c>
       <c r="D55" t="s">
-        <v>213</v>
+        <v>127</v>
       </c>
       <c r="E55" t="s">
-        <v>214</v>
-      </c>
-      <c r="F55" t="s">
-        <v>215</v>
-      </c>
-      <c r="G55" t="s">
-        <v>16</v>
-      </c>
-      <c r="H55">
-        <v>32</v>
+        <v>128</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I55">
         <v>389</v>

</xml_diff>